<commit_message>
viewloader 클래스 수정 전.
</commit_message>
<xml_diff>
--- a/Doc/XmlDataDocument_170601_dmgdensity변경.xlsx
+++ b/Doc/XmlDataDocument_170601_dmgdensity변경.xlsx
@@ -125,7 +125,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1232" uniqueCount="649">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1232" uniqueCount="650">
   <si>
     <t>hero</t>
   </si>
@@ -2428,6 +2428,10 @@
   </si>
   <si>
     <t>당시주요e갯수</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ingame</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2987,7 +2991,7 @@
         <name val="맑은 고딕"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="177" formatCode="0.0_ "/>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -3005,7 +3009,7 @@
         <name val="맑은 고딕"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="177" formatCode="0.0_ "/>
     </dxf>
     <dxf>
       <font>
@@ -4568,13 +4572,13 @@
     <tableColumn id="20" uniqueName="20" name="전체능력" dataDxfId="3">
       <calculatedColumnFormula>S2/2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" uniqueName="21" name="부분능력" dataDxfId="0">
+    <tableColumn id="21" uniqueName="21" name="부분능력" dataDxfId="2">
       <calculatedColumnFormula>S2*W2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="23" uniqueName="23" name="부분크리능력" dataDxfId="2">
+    <tableColumn id="23" uniqueName="23" name="부분크리능력" dataDxfId="1">
       <calculatedColumnFormula>표8[[#This Row],[부분능력]]*2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="22" uniqueName="22" name="당시주요e갯수" dataDxfId="1"/>
+    <tableColumn id="22" uniqueName="22" name="당시주요e갯수" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4868,7 +4872,7 @@
   <dimension ref="A1:N51"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -6517,8 +6521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q115"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -6632,7 +6636,7 @@
         <v>150</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>10</v>
+        <v>649</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>149</v>
@@ -6679,7 +6683,7 @@
         <v>150</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>26</v>
+        <v>649</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>149</v>
@@ -6726,7 +6730,7 @@
         <v>150</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>13</v>
+        <v>649</v>
       </c>
       <c r="O4" s="1" t="s">
         <v>149</v>
@@ -6773,7 +6777,7 @@
         <v>150</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>15</v>
+        <v>649</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>149</v>
@@ -6820,7 +6824,7 @@
         <v>150</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>12</v>
+        <v>649</v>
       </c>
       <c r="O6" s="1" t="s">
         <v>149</v>
@@ -6867,7 +6871,7 @@
         <v>150</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>24</v>
+        <v>649</v>
       </c>
       <c r="O7" s="1" t="s">
         <v>149</v>
@@ -6913,7 +6917,7 @@
         <v>150</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>25</v>
+        <v>649</v>
       </c>
       <c r="O8" s="1" t="s">
         <v>149</v>
@@ -6959,7 +6963,7 @@
         <v>150</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>467</v>
+        <v>649</v>
       </c>
       <c r="O9" s="1" t="s">
         <v>149</v>
@@ -7005,7 +7009,7 @@
         <v>150</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>23</v>
+        <v>649</v>
       </c>
       <c r="O10" s="1" t="s">
         <v>149</v>
@@ -7051,7 +7055,7 @@
         <v>75</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>10</v>
+        <v>649</v>
       </c>
       <c r="O11" s="1" t="s">
         <v>135</v>
@@ -7098,7 +7102,7 @@
         <v>75</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>26</v>
+        <v>649</v>
       </c>
       <c r="O12" s="1" t="s">
         <v>135</v>
@@ -7145,7 +7149,7 @@
         <v>75</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>13</v>
+        <v>649</v>
       </c>
       <c r="O13" s="1" t="s">
         <v>135</v>
@@ -7192,7 +7196,7 @@
         <v>75</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>15</v>
+        <v>649</v>
       </c>
       <c r="O14" s="1" t="s">
         <v>135</v>
@@ -7239,7 +7243,7 @@
         <v>75</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>12</v>
+        <v>649</v>
       </c>
       <c r="O15" s="1" t="s">
         <v>135</v>
@@ -7286,7 +7290,7 @@
         <v>75</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>24</v>
+        <v>649</v>
       </c>
       <c r="O16" s="1" t="s">
         <v>135</v>
@@ -7332,7 +7336,7 @@
         <v>75</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>25</v>
+        <v>649</v>
       </c>
       <c r="O17" s="1" t="s">
         <v>135</v>
@@ -7378,7 +7382,7 @@
         <v>75</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>467</v>
+        <v>649</v>
       </c>
       <c r="O18" s="1" t="s">
         <v>135</v>
@@ -7424,7 +7428,7 @@
         <v>75</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>23</v>
+        <v>649</v>
       </c>
       <c r="O19" s="1" t="s">
         <v>135</v>
@@ -7472,7 +7476,7 @@
         <v>0</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>9</v>
+        <v>649</v>
       </c>
       <c r="O20" s="1" t="s">
         <v>148</v>
@@ -7521,7 +7525,7 @@
         <v>0</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>9</v>
+        <v>649</v>
       </c>
       <c r="O21" s="1" t="s">
         <v>148</v>
@@ -7570,7 +7574,7 @@
         <v>0</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>9</v>
+        <v>649</v>
       </c>
       <c r="O22" s="1" t="s">
         <v>148</v>
@@ -7619,7 +7623,7 @@
         <v>0</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>9</v>
+        <v>649</v>
       </c>
       <c r="O23" s="1" t="s">
         <v>148</v>
@@ -7668,7 +7672,7 @@
         <v>0</v>
       </c>
       <c r="N24" s="1" t="s">
-        <v>9</v>
+        <v>649</v>
       </c>
       <c r="O24" s="1" t="s">
         <v>148</v>
@@ -7716,7 +7720,7 @@
         <v>0</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>9</v>
+        <v>649</v>
       </c>
       <c r="O25" s="1" t="s">
         <v>148</v>
@@ -7764,7 +7768,7 @@
         <v>0</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>9</v>
+        <v>649</v>
       </c>
       <c r="O26" s="1" t="s">
         <v>148</v>
@@ -7812,7 +7816,7 @@
         <v>0</v>
       </c>
       <c r="N27" s="1" t="s">
-        <v>9</v>
+        <v>649</v>
       </c>
       <c r="O27" s="1" t="s">
         <v>148</v>
@@ -10897,8 +10901,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:G8"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -11634,7 +11638,7 @@
   <dimension ref="A1:P61"/>
   <sheetViews>
     <sheetView showZeros="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="11.25"/>
@@ -13410,7 +13414,7 @@
   <dimension ref="A1:Z47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+      <selection activeCell="T7" sqref="T7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
@@ -13594,14 +13598,14 @@
       </c>
       <c r="U3" s="31">
         <f t="shared" si="0"/>
-        <v>5.0250000000000004</v>
+        <v>15.075000000000001</v>
       </c>
       <c r="V3" s="31">
         <f>표8[[#This Row],[부분능력]]*2</f>
-        <v>10.050000000000001</v>
+        <v>30.150000000000002</v>
       </c>
       <c r="W3" s="29">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Y3" s="52" t="s">
         <v>312</v>
@@ -13642,14 +13646,14 @@
       </c>
       <c r="U4" s="31">
         <f t="shared" si="0"/>
-        <v>5.0250000000000004</v>
+        <v>15.075000000000001</v>
       </c>
       <c r="V4" s="31">
         <f>표8[[#This Row],[부분능력]]*2</f>
-        <v>10.050000000000001</v>
+        <v>30.150000000000002</v>
       </c>
       <c r="W4" s="29">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Y4" s="54" t="s">
         <v>314</v>
@@ -13702,14 +13706,14 @@
       </c>
       <c r="U5" s="31">
         <f t="shared" si="0"/>
-        <v>5.0250000000000004</v>
+        <v>15.075000000000001</v>
       </c>
       <c r="V5" s="31">
         <f>표8[[#This Row],[부분능력]]*2</f>
-        <v>10.050000000000001</v>
+        <v>30.150000000000002</v>
       </c>
       <c r="W5" s="29">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Y5" s="56" t="s">
         <v>316</v>
@@ -13762,14 +13766,14 @@
       </c>
       <c r="U6" s="31">
         <f t="shared" si="0"/>
-        <v>5.0250000000000004</v>
+        <v>15.075000000000001</v>
       </c>
       <c r="V6" s="31">
         <f>표8[[#This Row],[부분능력]]*2</f>
-        <v>10.050000000000001</v>
+        <v>30.150000000000002</v>
       </c>
       <c r="W6" s="29">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:26">
@@ -13816,14 +13820,14 @@
       </c>
       <c r="U7" s="31">
         <f t="shared" si="0"/>
-        <v>5.0250000000000004</v>
+        <v>15.075000000000001</v>
       </c>
       <c r="V7" s="31">
         <f>표8[[#This Row],[부분능력]]*2</f>
-        <v>10.050000000000001</v>
+        <v>30.150000000000002</v>
       </c>
       <c r="W7" s="29">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:26">
@@ -13870,14 +13874,14 @@
       </c>
       <c r="U8" s="31">
         <f t="shared" si="0"/>
-        <v>5.0250000000000004</v>
+        <v>15.075000000000001</v>
       </c>
       <c r="V8" s="31">
         <f>표8[[#This Row],[부분능력]]*2</f>
-        <v>10.050000000000001</v>
+        <v>30.150000000000002</v>
       </c>
       <c r="W8" s="29">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:26">
@@ -13900,7 +13904,7 @@
         <v>323</v>
       </c>
       <c r="G9" s="29">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="H9" s="32"/>
       <c r="I9" s="32"/>
@@ -13924,14 +13928,14 @@
       </c>
       <c r="U9" s="31">
         <f t="shared" si="0"/>
-        <v>5.0250000000000004</v>
+        <v>15.075000000000001</v>
       </c>
       <c r="V9" s="31">
         <f>표8[[#This Row],[부분능력]]*2</f>
-        <v>10.050000000000001</v>
+        <v>30.150000000000002</v>
       </c>
       <c r="W9" s="29">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:26">
@@ -13966,14 +13970,14 @@
       </c>
       <c r="U10" s="31">
         <f t="shared" si="0"/>
-        <v>5.0250000000000004</v>
+        <v>15.075000000000001</v>
       </c>
       <c r="V10" s="31">
         <f>표8[[#This Row],[부분능력]]*2</f>
-        <v>10.050000000000001</v>
+        <v>30.150000000000002</v>
       </c>
       <c r="W10" s="29">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:26">
@@ -14009,14 +14013,14 @@
       </c>
       <c r="U11" s="31">
         <f t="shared" si="0"/>
-        <v>5.0250000000000004</v>
+        <v>15.075000000000001</v>
       </c>
       <c r="V11" s="31">
         <f>표8[[#This Row],[부분능력]]*2</f>
-        <v>10.050000000000001</v>
+        <v>30.150000000000002</v>
       </c>
       <c r="W11" s="29">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:26">
@@ -14054,14 +14058,14 @@
       </c>
       <c r="U12" s="31">
         <f t="shared" si="0"/>
-        <v>6.1416666666666666</v>
+        <v>18.425000000000001</v>
       </c>
       <c r="V12" s="31">
         <f>표8[[#This Row],[부분능력]]*2</f>
-        <v>12.283333333333333</v>
+        <v>36.85</v>
       </c>
       <c r="W12" s="29">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:26">
@@ -14099,14 +14103,14 @@
       </c>
       <c r="U13" s="31">
         <f t="shared" si="0"/>
-        <v>6.1416666666666666</v>
+        <v>18.425000000000001</v>
       </c>
       <c r="V13" s="31">
         <f>표8[[#This Row],[부분능력]]*2</f>
-        <v>12.283333333333333</v>
+        <v>36.85</v>
       </c>
       <c r="W13" s="29">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:26">
@@ -14144,14 +14148,14 @@
       </c>
       <c r="U14" s="31">
         <f t="shared" si="0"/>
-        <v>6.1416666666666666</v>
+        <v>18.425000000000001</v>
       </c>
       <c r="V14" s="31">
         <f>표8[[#This Row],[부분능력]]*2</f>
-        <v>12.283333333333333</v>
+        <v>36.85</v>
       </c>
       <c r="W14" s="29">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:26">
@@ -14189,14 +14193,14 @@
       </c>
       <c r="U15" s="31">
         <f t="shared" si="0"/>
-        <v>6.1416666666666666</v>
+        <v>18.425000000000001</v>
       </c>
       <c r="V15" s="31">
         <f>표8[[#This Row],[부분능력]]*2</f>
-        <v>12.283333333333333</v>
+        <v>36.85</v>
       </c>
       <c r="W15" s="29">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:26">
@@ -14234,14 +14238,14 @@
       </c>
       <c r="U16" s="31">
         <f t="shared" si="0"/>
-        <v>6.1416666666666666</v>
+        <v>18.425000000000001</v>
       </c>
       <c r="V16" s="31">
         <f>표8[[#This Row],[부분능력]]*2</f>
-        <v>12.283333333333333</v>
+        <v>36.85</v>
       </c>
       <c r="W16" s="29">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:23">
@@ -14279,14 +14283,14 @@
       </c>
       <c r="U17" s="31">
         <f t="shared" si="0"/>
-        <v>6.1416666666666666</v>
+        <v>18.425000000000001</v>
       </c>
       <c r="V17" s="31">
         <f>표8[[#This Row],[부분능력]]*2</f>
-        <v>12.283333333333333</v>
+        <v>36.85</v>
       </c>
       <c r="W17" s="29">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:23">
@@ -14324,14 +14328,14 @@
       </c>
       <c r="U18" s="31">
         <f t="shared" si="0"/>
-        <v>12.525000000000002</v>
+        <v>62.625000000000014</v>
       </c>
       <c r="V18" s="31">
         <f>표8[[#This Row],[부분능력]]*2</f>
-        <v>25.050000000000004</v>
+        <v>125.25000000000003</v>
       </c>
       <c r="W18" s="29">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:23">
@@ -14369,14 +14373,14 @@
       </c>
       <c r="U19" s="31">
         <f t="shared" si="0"/>
-        <v>12.525000000000002</v>
+        <v>62.625000000000014</v>
       </c>
       <c r="V19" s="31">
         <f>표8[[#This Row],[부분능력]]*2</f>
-        <v>25.050000000000004</v>
+        <v>125.25000000000003</v>
       </c>
       <c r="W19" s="29">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:23">
@@ -14414,14 +14418,14 @@
       </c>
       <c r="U20" s="31">
         <f t="shared" si="0"/>
-        <v>12.525000000000002</v>
+        <v>62.625000000000014</v>
       </c>
       <c r="V20" s="31">
         <f>표8[[#This Row],[부분능력]]*2</f>
-        <v>25.050000000000004</v>
+        <v>125.25000000000003</v>
       </c>
       <c r="W20" s="29">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:23">
@@ -14459,14 +14463,14 @@
       </c>
       <c r="U21" s="31">
         <f t="shared" si="0"/>
-        <v>12.525000000000002</v>
+        <v>62.625000000000014</v>
       </c>
       <c r="V21" s="31">
         <f>표8[[#This Row],[부분능력]]*2</f>
-        <v>25.050000000000004</v>
+        <v>125.25000000000003</v>
       </c>
       <c r="W21" s="29">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:23">
@@ -14504,14 +14508,14 @@
       </c>
       <c r="U22" s="31">
         <f t="shared" si="0"/>
-        <v>12.525000000000002</v>
+        <v>62.625000000000014</v>
       </c>
       <c r="V22" s="31">
         <f>표8[[#This Row],[부분능력]]*2</f>
-        <v>25.050000000000004</v>
+        <v>125.25000000000003</v>
       </c>
       <c r="W22" s="29">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:23">
@@ -14549,14 +14553,14 @@
       </c>
       <c r="U23" s="31">
         <f t="shared" si="0"/>
-        <v>12.525000000000002</v>
+        <v>62.625000000000014</v>
       </c>
       <c r="V23" s="31">
         <f>표8[[#This Row],[부분능력]]*2</f>
-        <v>25.050000000000004</v>
+        <v>125.25000000000003</v>
       </c>
       <c r="W23" s="29">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:23">
@@ -14594,14 +14598,14 @@
       </c>
       <c r="U24" s="31">
         <f t="shared" si="0"/>
-        <v>12.525000000000002</v>
+        <v>62.625000000000014</v>
       </c>
       <c r="V24" s="31">
         <f>표8[[#This Row],[부분능력]]*2</f>
-        <v>25.050000000000004</v>
+        <v>125.25000000000003</v>
       </c>
       <c r="W24" s="29">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:23">
@@ -14639,14 +14643,14 @@
       </c>
       <c r="U25" s="31">
         <f t="shared" si="0"/>
-        <v>12.525000000000002</v>
+        <v>62.625000000000014</v>
       </c>
       <c r="V25" s="31">
         <f>표8[[#This Row],[부분능력]]*2</f>
-        <v>25.050000000000004</v>
+        <v>125.25000000000003</v>
       </c>
       <c r="W25" s="29">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:23">
@@ -14684,14 +14688,14 @@
       </c>
       <c r="U26" s="31">
         <f t="shared" si="0"/>
-        <v>12.525000000000002</v>
+        <v>62.625000000000014</v>
       </c>
       <c r="V26" s="31">
         <f>표8[[#This Row],[부분능력]]*2</f>
-        <v>25.050000000000004</v>
+        <v>125.25000000000003</v>
       </c>
       <c r="W26" s="29">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:23">
@@ -14729,14 +14733,14 @@
       </c>
       <c r="U27" s="31">
         <f t="shared" si="0"/>
-        <v>15.308333333333335</v>
+        <v>76.541666666666671</v>
       </c>
       <c r="V27" s="31">
         <f>표8[[#This Row],[부분능력]]*2</f>
-        <v>30.616666666666671</v>
+        <v>153.08333333333334</v>
       </c>
       <c r="W27" s="29">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:23">
@@ -14774,14 +14778,14 @@
       </c>
       <c r="U28" s="31">
         <f t="shared" si="0"/>
-        <v>15.308333333333335</v>
+        <v>76.541666666666671</v>
       </c>
       <c r="V28" s="31">
         <f>표8[[#This Row],[부분능력]]*2</f>
-        <v>30.616666666666671</v>
+        <v>153.08333333333334</v>
       </c>
       <c r="W28" s="29">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="29" spans="1:23">
@@ -14819,14 +14823,14 @@
       </c>
       <c r="U29" s="31">
         <f t="shared" si="0"/>
-        <v>15.308333333333335</v>
+        <v>76.541666666666671</v>
       </c>
       <c r="V29" s="31">
         <f>표8[[#This Row],[부분능력]]*2</f>
-        <v>30.616666666666671</v>
+        <v>153.08333333333334</v>
       </c>
       <c r="W29" s="29">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="30" spans="1:23">
@@ -14864,14 +14868,14 @@
       </c>
       <c r="U30" s="31">
         <f t="shared" si="0"/>
-        <v>15.308333333333335</v>
+        <v>76.541666666666671</v>
       </c>
       <c r="V30" s="31">
         <f>표8[[#This Row],[부분능력]]*2</f>
-        <v>30.616666666666671</v>
+        <v>153.08333333333334</v>
       </c>
       <c r="W30" s="29">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="31" spans="1:23">
@@ -14909,14 +14913,14 @@
       </c>
       <c r="U31" s="31">
         <f t="shared" si="0"/>
-        <v>15.308333333333335</v>
+        <v>76.541666666666671</v>
       </c>
       <c r="V31" s="31">
         <f>표8[[#This Row],[부분능력]]*2</f>
-        <v>30.616666666666671</v>
+        <v>153.08333333333334</v>
       </c>
       <c r="W31" s="29">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="32" spans="1:23">
@@ -14954,14 +14958,14 @@
       </c>
       <c r="U32" s="31">
         <f t="shared" si="0"/>
-        <v>15.308333333333335</v>
+        <v>76.541666666666671</v>
       </c>
       <c r="V32" s="31">
         <f>표8[[#This Row],[부분능력]]*2</f>
-        <v>30.616666666666671</v>
+        <v>153.08333333333334</v>
       </c>
       <c r="W32" s="29">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="33" spans="1:23">
@@ -14999,14 +15003,14 @@
       </c>
       <c r="U33" s="31">
         <f t="shared" si="0"/>
-        <v>46.8</v>
+        <v>140.39999999999998</v>
       </c>
       <c r="V33" s="31">
         <f>표8[[#This Row],[부분능력]]*2</f>
-        <v>93.6</v>
+        <v>280.79999999999995</v>
       </c>
       <c r="W33" s="29">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="34" spans="1:23">
@@ -15044,14 +15048,14 @@
       </c>
       <c r="U34" s="31">
         <f t="shared" si="0"/>
-        <v>46.8</v>
+        <v>140.39999999999998</v>
       </c>
       <c r="V34" s="31">
         <f>표8[[#This Row],[부분능력]]*2</f>
-        <v>93.6</v>
+        <v>280.79999999999995</v>
       </c>
       <c r="W34" s="29">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="35" spans="1:23">
@@ -15089,14 +15093,14 @@
       </c>
       <c r="U35" s="31">
         <f t="shared" si="0"/>
-        <v>46.8</v>
+        <v>140.39999999999998</v>
       </c>
       <c r="V35" s="31">
         <f>표8[[#This Row],[부분능력]]*2</f>
-        <v>93.6</v>
+        <v>280.79999999999995</v>
       </c>
       <c r="W35" s="29">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="36" spans="1:23">
@@ -15134,14 +15138,14 @@
       </c>
       <c r="U36" s="31">
         <f t="shared" si="0"/>
-        <v>46.8</v>
+        <v>140.39999999999998</v>
       </c>
       <c r="V36" s="31">
         <f>표8[[#This Row],[부분능력]]*2</f>
-        <v>93.6</v>
+        <v>280.79999999999995</v>
       </c>
       <c r="W36" s="29">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="37" spans="1:23">
@@ -15179,14 +15183,14 @@
       </c>
       <c r="U37" s="31">
         <f t="shared" si="0"/>
-        <v>46.8</v>
+        <v>140.39999999999998</v>
       </c>
       <c r="V37" s="31">
         <f>표8[[#This Row],[부분능력]]*2</f>
-        <v>93.6</v>
+        <v>280.79999999999995</v>
       </c>
       <c r="W37" s="29">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="38" spans="1:23">
@@ -15224,14 +15228,14 @@
       </c>
       <c r="U38" s="31">
         <f t="shared" si="0"/>
-        <v>46.8</v>
+        <v>140.39999999999998</v>
       </c>
       <c r="V38" s="31">
         <f>표8[[#This Row],[부분능력]]*2</f>
-        <v>93.6</v>
+        <v>280.79999999999995</v>
       </c>
       <c r="W38" s="29">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="39" spans="1:23">
@@ -15269,14 +15273,14 @@
       </c>
       <c r="U39" s="31">
         <f t="shared" si="0"/>
-        <v>46.8</v>
+        <v>140.39999999999998</v>
       </c>
       <c r="V39" s="31">
         <f>표8[[#This Row],[부분능력]]*2</f>
-        <v>93.6</v>
+        <v>280.79999999999995</v>
       </c>
       <c r="W39" s="29">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="40" spans="1:23">
@@ -15314,14 +15318,14 @@
       </c>
       <c r="U40" s="31">
         <f t="shared" si="0"/>
-        <v>46.8</v>
+        <v>140.39999999999998</v>
       </c>
       <c r="V40" s="31">
         <f>표8[[#This Row],[부분능력]]*2</f>
-        <v>93.6</v>
+        <v>280.79999999999995</v>
       </c>
       <c r="W40" s="29">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="41" spans="1:23">
@@ -15359,14 +15363,14 @@
       </c>
       <c r="U41" s="31">
         <f t="shared" si="0"/>
-        <v>46.8</v>
+        <v>140.39999999999998</v>
       </c>
       <c r="V41" s="31">
         <f>표8[[#This Row],[부분능력]]*2</f>
-        <v>93.6</v>
+        <v>280.79999999999995</v>
       </c>
       <c r="W41" s="29">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="42" spans="1:23">
@@ -15404,14 +15408,14 @@
       </c>
       <c r="U42" s="31">
         <f t="shared" si="0"/>
-        <v>57.199999999999989</v>
+        <v>171.59999999999997</v>
       </c>
       <c r="V42" s="31">
         <f>표8[[#This Row],[부분능력]]*2</f>
-        <v>114.39999999999998</v>
+        <v>343.19999999999993</v>
       </c>
       <c r="W42" s="29">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="43" spans="1:23">
@@ -15449,14 +15453,14 @@
       </c>
       <c r="U43" s="31">
         <f t="shared" si="0"/>
-        <v>57.199999999999989</v>
+        <v>171.59999999999997</v>
       </c>
       <c r="V43" s="31">
         <f>표8[[#This Row],[부분능력]]*2</f>
-        <v>114.39999999999998</v>
+        <v>343.19999999999993</v>
       </c>
       <c r="W43" s="29">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="44" spans="1:23">
@@ -15494,14 +15498,14 @@
       </c>
       <c r="U44" s="31">
         <f t="shared" si="0"/>
-        <v>57.199999999999989</v>
+        <v>171.59999999999997</v>
       </c>
       <c r="V44" s="31">
         <f>표8[[#This Row],[부분능력]]*2</f>
-        <v>114.39999999999998</v>
+        <v>343.19999999999993</v>
       </c>
       <c r="W44" s="29">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="45" spans="1:23">
@@ -15539,14 +15543,14 @@
       </c>
       <c r="U45" s="31">
         <f t="shared" si="0"/>
-        <v>57.199999999999989</v>
+        <v>171.59999999999997</v>
       </c>
       <c r="V45" s="31">
         <f>표8[[#This Row],[부분능력]]*2</f>
-        <v>114.39999999999998</v>
+        <v>343.19999999999993</v>
       </c>
       <c r="W45" s="29">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="46" spans="1:23">
@@ -15584,14 +15588,14 @@
       </c>
       <c r="U46" s="31">
         <f t="shared" si="0"/>
-        <v>57.199999999999989</v>
+        <v>171.59999999999997</v>
       </c>
       <c r="V46" s="31">
         <f>표8[[#This Row],[부분능력]]*2</f>
-        <v>114.39999999999998</v>
+        <v>343.19999999999993</v>
       </c>
       <c r="W46" s="29">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="47" spans="1:23">
@@ -15629,14 +15633,14 @@
       </c>
       <c r="U47" s="31">
         <f t="shared" si="0"/>
-        <v>57.199999999999989</v>
+        <v>171.59999999999997</v>
       </c>
       <c r="V47" s="31">
         <f>표8[[#This Row],[부분능력]]*2</f>
-        <v>114.39999999999998</v>
+        <v>343.19999999999993</v>
       </c>
       <c r="W47" s="29">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>